<commit_message>
overhaul of vivid_epi structure
</commit_message>
<xml_diff>
--- a/internal_datamap_files/liftPR_internal_covar_map.xlsx
+++ b/internal_datamap_files/liftPR_internal_covar_map.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28410"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NFB/Documents/GitHub/VivID_Epi/internal_datamap_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/internal_datamap_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D8D744-0D15-D547-ABAF-E6DC26AB92E1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4720" windowWidth="25540" windowHeight="20780" activeTab="1"/>
+    <workbookView xWindow="5340" yWindow="460" windowWidth="20200" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
     <sheet name="covar_names_labels" sheetId="1" r:id="rId2"/>
     <sheet name="cmpr_M_F_biocovar" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -2911,9 +2912,6 @@
     <t>extra -- don't need</t>
   </si>
   <si>
-    <t>divide by 1e5</t>
-  </si>
-  <si>
     <t>lubridate</t>
   </si>
   <si>
@@ -3146,12 +3144,15 @@
   </si>
   <si>
     <t>continuous, but manually recode -- 96 on premises</t>
+  </si>
+  <si>
+    <t>divide by 1e6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4106,7 +4107,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A8:H23"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
@@ -4286,11 +4287,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E538"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4313,7 +4314,7 @@
         <v>957</v>
       </c>
       <c r="E1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -4484,7 +4485,7 @@
         <v>956</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>960</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -4501,7 +4502,7 @@
         <v>956</v>
       </c>
       <c r="E14" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -4518,7 +4519,7 @@
         <v>956</v>
       </c>
       <c r="E15" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -4552,7 +4553,7 @@
         <v>956</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -4569,7 +4570,7 @@
         <v>956</v>
       </c>
       <c r="E18" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -4586,7 +4587,7 @@
         <v>956</v>
       </c>
       <c r="E19" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -4603,7 +4604,7 @@
         <v>956</v>
       </c>
       <c r="E20" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -4620,7 +4621,7 @@
         <v>956</v>
       </c>
       <c r="E21" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -4637,7 +4638,7 @@
         <v>956</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -4671,7 +4672,7 @@
         <v>955</v>
       </c>
       <c r="E24" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -4688,7 +4689,7 @@
         <v>956</v>
       </c>
       <c r="E25" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -4705,7 +4706,7 @@
         <v>956</v>
       </c>
       <c r="E26" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -4722,7 +4723,7 @@
         <v>956</v>
       </c>
       <c r="E27" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -4736,10 +4737,10 @@
         <v>956</v>
       </c>
       <c r="D28" t="s">
+        <v>965</v>
+      </c>
+      <c r="E28" t="s">
         <v>966</v>
-      </c>
-      <c r="E28" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -4756,7 +4757,7 @@
         <v>956</v>
       </c>
       <c r="E29" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -4770,10 +4771,10 @@
         <v>956</v>
       </c>
       <c r="D30" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E30" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -4787,10 +4788,10 @@
         <v>956</v>
       </c>
       <c r="D31" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E31" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -4804,10 +4805,10 @@
         <v>956</v>
       </c>
       <c r="D32" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E32" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -4824,7 +4825,7 @@
         <v>956</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -4855,7 +4856,7 @@
         <v>956</v>
       </c>
       <c r="E35" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -4872,7 +4873,7 @@
         <v>956</v>
       </c>
       <c r="E36" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -4889,7 +4890,7 @@
         <v>956</v>
       </c>
       <c r="E37" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -4906,7 +4907,7 @@
         <v>956</v>
       </c>
       <c r="E38" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -4923,7 +4924,7 @@
         <v>956</v>
       </c>
       <c r="E39" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -4954,7 +4955,7 @@
         <v>956</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -4968,7 +4969,7 @@
         <v>956</v>
       </c>
       <c r="D42" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -4985,7 +4986,7 @@
         <v>956</v>
       </c>
       <c r="E43" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -5002,7 +5003,7 @@
         <v>956</v>
       </c>
       <c r="E44" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -5019,7 +5020,7 @@
         <v>956</v>
       </c>
       <c r="E45" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -5036,7 +5037,7 @@
         <v>956</v>
       </c>
       <c r="E46" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -5053,7 +5054,7 @@
         <v>956</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -5182,7 +5183,7 @@
         <v>955</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -5199,7 +5200,7 @@
         <v>955</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -5216,7 +5217,7 @@
         <v>955</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -5233,7 +5234,7 @@
         <v>956</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -5264,7 +5265,7 @@
         <v>956</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -5296,7 +5297,7 @@
         <v>956</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -5358,7 +5359,7 @@
         <v>956</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -5372,10 +5373,10 @@
         <v>956</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -5392,7 +5393,7 @@
         <v>956</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -5409,7 +5410,7 @@
         <v>956</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -5426,7 +5427,7 @@
         <v>956</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -5443,7 +5444,7 @@
         <v>956</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -5460,7 +5461,7 @@
         <v>956</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
@@ -5477,7 +5478,7 @@
         <v>956</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -5494,7 +5495,7 @@
         <v>956</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
@@ -5511,7 +5512,7 @@
         <v>956</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
@@ -5528,7 +5529,7 @@
         <v>956</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
@@ -5560,7 +5561,7 @@
         <v>956</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -5577,7 +5578,7 @@
         <v>956</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -5609,7 +5610,7 @@
         <v>956</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -5626,7 +5627,7 @@
         <v>956</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -5643,7 +5644,7 @@
         <v>956</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -5660,7 +5661,7 @@
         <v>956</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -5677,7 +5678,7 @@
         <v>956</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -5694,7 +5695,7 @@
         <v>956</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -5711,7 +5712,7 @@
         <v>956</v>
       </c>
       <c r="E88" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -5728,7 +5729,7 @@
         <v>956</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -5745,7 +5746,7 @@
         <v>956</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -5762,7 +5763,7 @@
         <v>956</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -5779,7 +5780,7 @@
         <v>956</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -5796,7 +5797,7 @@
         <v>956</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -5813,7 +5814,7 @@
         <v>956</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -5830,7 +5831,7 @@
         <v>956</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -5847,7 +5848,7 @@
         <v>956</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -5864,7 +5865,7 @@
         <v>956</v>
       </c>
       <c r="E97" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -5986,7 +5987,7 @@
         <v>956</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -6018,7 +6019,7 @@
         <v>956</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -6035,7 +6036,7 @@
         <v>956</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -6052,7 +6053,7 @@
         <v>956</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -6069,7 +6070,7 @@
         <v>956</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -6086,7 +6087,7 @@
         <v>956</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -6103,7 +6104,7 @@
         <v>956</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -6120,7 +6121,7 @@
         <v>956</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -6137,7 +6138,7 @@
         <v>956</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -6154,7 +6155,7 @@
         <v>956</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -6171,7 +6172,7 @@
         <v>956</v>
       </c>
       <c r="E116" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -6188,7 +6189,7 @@
         <v>956</v>
       </c>
       <c r="E117" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -6235,7 +6236,7 @@
         <v>956</v>
       </c>
       <c r="E120" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
@@ -6252,7 +6253,7 @@
         <v>956</v>
       </c>
       <c r="E121" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
@@ -6269,7 +6270,7 @@
         <v>956</v>
       </c>
       <c r="E122" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
@@ -6286,7 +6287,7 @@
         <v>956</v>
       </c>
       <c r="E123" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
@@ -6303,7 +6304,7 @@
         <v>956</v>
       </c>
       <c r="E124" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
@@ -6320,7 +6321,7 @@
         <v>956</v>
       </c>
       <c r="E125" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
@@ -6337,7 +6338,7 @@
         <v>956</v>
       </c>
       <c r="E126" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -6354,7 +6355,7 @@
         <v>956</v>
       </c>
       <c r="E127" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
@@ -6371,7 +6372,7 @@
         <v>956</v>
       </c>
       <c r="E128" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -6388,7 +6389,7 @@
         <v>956</v>
       </c>
       <c r="E129" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
@@ -6405,7 +6406,7 @@
         <v>956</v>
       </c>
       <c r="E130" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
@@ -6437,7 +6438,7 @@
         <v>956</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -6454,7 +6455,7 @@
         <v>956</v>
       </c>
       <c r="E133" s="7" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -6471,7 +6472,7 @@
         <v>956</v>
       </c>
       <c r="E134" s="7" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
@@ -6485,10 +6486,10 @@
         <v>956</v>
       </c>
       <c r="D135" s="7" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="E135" s="7" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -6505,7 +6506,7 @@
         <v>956</v>
       </c>
       <c r="E136" s="9" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -6522,7 +6523,7 @@
         <v>956</v>
       </c>
       <c r="E137" s="11" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
@@ -6539,7 +6540,7 @@
         <v>956</v>
       </c>
       <c r="E138" s="11" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
@@ -6556,7 +6557,7 @@
         <v>955</v>
       </c>
       <c r="E139" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -6573,7 +6574,7 @@
         <v>955</v>
       </c>
       <c r="E140" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -6590,7 +6591,7 @@
         <v>955</v>
       </c>
       <c r="E141" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
@@ -6607,7 +6608,7 @@
         <v>955</v>
       </c>
       <c r="E142" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
@@ -6624,7 +6625,7 @@
         <v>955</v>
       </c>
       <c r="E143" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
@@ -6641,7 +6642,7 @@
         <v>955</v>
       </c>
       <c r="E144" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
@@ -6658,7 +6659,7 @@
         <v>955</v>
       </c>
       <c r="E145" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
@@ -6675,7 +6676,7 @@
         <v>955</v>
       </c>
       <c r="E146" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
@@ -6692,7 +6693,7 @@
         <v>955</v>
       </c>
       <c r="E147" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
@@ -6709,7 +6710,7 @@
         <v>955</v>
       </c>
       <c r="E148" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -6726,7 +6727,7 @@
         <v>955</v>
       </c>
       <c r="E149" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
@@ -6743,7 +6744,7 @@
         <v>955</v>
       </c>
       <c r="E150" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
@@ -6760,7 +6761,7 @@
         <v>955</v>
       </c>
       <c r="E151" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
@@ -6777,7 +6778,7 @@
         <v>955</v>
       </c>
       <c r="E152" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
@@ -6794,7 +6795,7 @@
         <v>955</v>
       </c>
       <c r="E153" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
@@ -6811,7 +6812,7 @@
         <v>955</v>
       </c>
       <c r="E154" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
@@ -6828,7 +6829,7 @@
         <v>955</v>
       </c>
       <c r="E155" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
@@ -6845,7 +6846,7 @@
         <v>955</v>
       </c>
       <c r="E156" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
@@ -6862,7 +6863,7 @@
         <v>955</v>
       </c>
       <c r="E157" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
@@ -6879,7 +6880,7 @@
         <v>955</v>
       </c>
       <c r="E158" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
@@ -6896,7 +6897,7 @@
         <v>955</v>
       </c>
       <c r="E159" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
@@ -6913,7 +6914,7 @@
         <v>955</v>
       </c>
       <c r="E160" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
@@ -6930,7 +6931,7 @@
         <v>955</v>
       </c>
       <c r="E161" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
@@ -6947,7 +6948,7 @@
         <v>955</v>
       </c>
       <c r="E162" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
@@ -6964,7 +6965,7 @@
         <v>955</v>
       </c>
       <c r="E163" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
@@ -6981,7 +6982,7 @@
         <v>955</v>
       </c>
       <c r="E164" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
@@ -6998,7 +6999,7 @@
         <v>955</v>
       </c>
       <c r="E165" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.2">
@@ -7015,7 +7016,7 @@
         <v>955</v>
       </c>
       <c r="E166" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
@@ -7032,7 +7033,7 @@
         <v>955</v>
       </c>
       <c r="E167" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
@@ -7049,7 +7050,7 @@
         <v>955</v>
       </c>
       <c r="E168" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
@@ -7066,7 +7067,7 @@
         <v>955</v>
       </c>
       <c r="E169" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
@@ -7083,7 +7084,7 @@
         <v>955</v>
       </c>
       <c r="E170" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
@@ -7100,7 +7101,7 @@
         <v>955</v>
       </c>
       <c r="E171" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.2">
@@ -7117,7 +7118,7 @@
         <v>955</v>
       </c>
       <c r="E172" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
@@ -7134,7 +7135,7 @@
         <v>955</v>
       </c>
       <c r="E173" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
@@ -7151,7 +7152,7 @@
         <v>955</v>
       </c>
       <c r="E174" s="12" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
@@ -7168,7 +7169,7 @@
         <v>956</v>
       </c>
       <c r="E175" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
@@ -7185,7 +7186,7 @@
         <v>956</v>
       </c>
       <c r="E176" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
@@ -7202,7 +7203,7 @@
         <v>956</v>
       </c>
       <c r="E177" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
@@ -7219,7 +7220,7 @@
         <v>956</v>
       </c>
       <c r="E178" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
@@ -7236,7 +7237,7 @@
         <v>956</v>
       </c>
       <c r="E179" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
@@ -7253,7 +7254,7 @@
         <v>956</v>
       </c>
       <c r="E180" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
@@ -7270,7 +7271,7 @@
         <v>956</v>
       </c>
       <c r="E181" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
@@ -7287,7 +7288,7 @@
         <v>956</v>
       </c>
       <c r="E182" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
@@ -7304,7 +7305,7 @@
         <v>956</v>
       </c>
       <c r="E183" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
@@ -7321,7 +7322,7 @@
         <v>956</v>
       </c>
       <c r="E184" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
@@ -7338,7 +7339,7 @@
         <v>956</v>
       </c>
       <c r="E185" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
@@ -7355,7 +7356,7 @@
         <v>956</v>
       </c>
       <c r="E186" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
@@ -7372,7 +7373,7 @@
         <v>956</v>
       </c>
       <c r="E187" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
@@ -7389,7 +7390,7 @@
         <v>956</v>
       </c>
       <c r="E188" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
@@ -7406,7 +7407,7 @@
         <v>956</v>
       </c>
       <c r="E189" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.2">
@@ -7423,7 +7424,7 @@
         <v>956</v>
       </c>
       <c r="E190" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
@@ -7440,7 +7441,7 @@
         <v>956</v>
       </c>
       <c r="E191" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
@@ -7457,7 +7458,7 @@
         <v>956</v>
       </c>
       <c r="E192" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
@@ -7474,7 +7475,7 @@
         <v>956</v>
       </c>
       <c r="E193" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
@@ -7491,7 +7492,7 @@
         <v>956</v>
       </c>
       <c r="E194" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
@@ -7508,7 +7509,7 @@
         <v>956</v>
       </c>
       <c r="E195" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
@@ -7525,7 +7526,7 @@
         <v>956</v>
       </c>
       <c r="E196" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
@@ -7542,7 +7543,7 @@
         <v>956</v>
       </c>
       <c r="E197" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
@@ -7559,7 +7560,7 @@
         <v>956</v>
       </c>
       <c r="E198" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
@@ -7576,7 +7577,7 @@
         <v>956</v>
       </c>
       <c r="E199" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
@@ -7593,7 +7594,7 @@
         <v>956</v>
       </c>
       <c r="E200" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
@@ -7610,7 +7611,7 @@
         <v>956</v>
       </c>
       <c r="E201" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
@@ -7627,7 +7628,7 @@
         <v>956</v>
       </c>
       <c r="E202" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
@@ -7644,7 +7645,7 @@
         <v>956</v>
       </c>
       <c r="E203" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
@@ -7661,7 +7662,7 @@
         <v>956</v>
       </c>
       <c r="E204" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
@@ -7678,7 +7679,7 @@
         <v>956</v>
       </c>
       <c r="E205" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
@@ -7695,7 +7696,7 @@
         <v>956</v>
       </c>
       <c r="E206" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
@@ -7712,7 +7713,7 @@
         <v>956</v>
       </c>
       <c r="E207" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
@@ -7729,7 +7730,7 @@
         <v>956</v>
       </c>
       <c r="E208" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
@@ -7746,7 +7747,7 @@
         <v>956</v>
       </c>
       <c r="E209" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
@@ -7763,7 +7764,7 @@
         <v>956</v>
       </c>
       <c r="E210" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
@@ -7780,7 +7781,7 @@
         <v>956</v>
       </c>
       <c r="E211" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
@@ -7797,7 +7798,7 @@
         <v>956</v>
       </c>
       <c r="E212" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.2">
@@ -7814,7 +7815,7 @@
         <v>956</v>
       </c>
       <c r="E213" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.2">
@@ -7831,7 +7832,7 @@
         <v>956</v>
       </c>
       <c r="E214" s="12" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
@@ -7848,7 +7849,7 @@
         <v>956</v>
       </c>
       <c r="E215" s="10" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
@@ -7865,7 +7866,7 @@
         <v>956</v>
       </c>
       <c r="E216" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
@@ -7882,7 +7883,7 @@
         <v>956</v>
       </c>
       <c r="E217" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
@@ -7899,7 +7900,7 @@
         <v>956</v>
       </c>
       <c r="E218" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
@@ -7930,7 +7931,7 @@
         <v>956</v>
       </c>
       <c r="E220" s="6" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
@@ -7947,7 +7948,7 @@
         <v>955</v>
       </c>
       <c r="E221" s="8" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
@@ -7964,7 +7965,7 @@
         <v>955</v>
       </c>
       <c r="E222" s="8" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
@@ -7981,7 +7982,7 @@
         <v>955</v>
       </c>
       <c r="E223" s="8" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
@@ -7998,7 +7999,7 @@
         <v>955</v>
       </c>
       <c r="E224" s="8" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.2">
@@ -8015,7 +8016,7 @@
         <v>956</v>
       </c>
       <c r="E225" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
@@ -8032,7 +8033,7 @@
         <v>956</v>
       </c>
       <c r="E226" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
@@ -8049,7 +8050,7 @@
         <v>956</v>
       </c>
       <c r="E227" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
@@ -8066,7 +8067,7 @@
         <v>956</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
@@ -8083,7 +8084,7 @@
         <v>956</v>
       </c>
       <c r="E229" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
@@ -8115,7 +8116,7 @@
         <v>956</v>
       </c>
       <c r="E231" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
@@ -8177,7 +8178,7 @@
         <v>956</v>
       </c>
       <c r="E235" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
@@ -8194,7 +8195,7 @@
         <v>956</v>
       </c>
       <c r="E236" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
@@ -8211,7 +8212,7 @@
         <v>956</v>
       </c>
       <c r="E237" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
@@ -8228,7 +8229,7 @@
         <v>956</v>
       </c>
       <c r="E238" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
@@ -8245,7 +8246,7 @@
         <v>956</v>
       </c>
       <c r="E239" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.2">
@@ -8262,7 +8263,7 @@
         <v>956</v>
       </c>
       <c r="E240" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.2">
@@ -8279,7 +8280,7 @@
         <v>956</v>
       </c>
       <c r="E241" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.2">
@@ -8296,7 +8297,7 @@
         <v>956</v>
       </c>
       <c r="E242" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.2">
@@ -8313,7 +8314,7 @@
         <v>956</v>
       </c>
       <c r="E243" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
@@ -8330,7 +8331,7 @@
         <v>956</v>
       </c>
       <c r="E244" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.2">
@@ -8362,7 +8363,7 @@
         <v>956</v>
       </c>
       <c r="E246" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.2">
@@ -8379,7 +8380,7 @@
         <v>956</v>
       </c>
       <c r="E247" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.2">
@@ -8396,7 +8397,7 @@
         <v>956</v>
       </c>
       <c r="E248" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.2">
@@ -8413,7 +8414,7 @@
         <v>956</v>
       </c>
       <c r="E249" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
@@ -8430,7 +8431,7 @@
         <v>956</v>
       </c>
       <c r="E250" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.2">
@@ -8447,7 +8448,7 @@
         <v>956</v>
       </c>
       <c r="E251" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
@@ -8464,7 +8465,7 @@
         <v>956</v>
       </c>
       <c r="E252" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
@@ -8481,7 +8482,7 @@
         <v>956</v>
       </c>
       <c r="E253" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.2">
@@ -8498,7 +8499,7 @@
         <v>956</v>
       </c>
       <c r="E254" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.2">
@@ -8515,7 +8516,7 @@
         <v>956</v>
       </c>
       <c r="E255" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.2">
@@ -8532,7 +8533,7 @@
         <v>956</v>
       </c>
       <c r="E256" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.2">
@@ -8549,7 +8550,7 @@
         <v>956</v>
       </c>
       <c r="E257" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.2">
@@ -8566,7 +8567,7 @@
         <v>956</v>
       </c>
       <c r="E258" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.2">
@@ -8583,7 +8584,7 @@
         <v>956</v>
       </c>
       <c r="E259" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.2">
@@ -8600,7 +8601,7 @@
         <v>956</v>
       </c>
       <c r="E260" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.2">
@@ -8617,7 +8618,7 @@
         <v>956</v>
       </c>
       <c r="E261" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.2">
@@ -8634,7 +8635,7 @@
         <v>956</v>
       </c>
       <c r="E262" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.2">
@@ -8651,7 +8652,7 @@
         <v>956</v>
       </c>
       <c r="E263" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.2">
@@ -8668,7 +8669,7 @@
         <v>956</v>
       </c>
       <c r="E264" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.2">
@@ -8685,7 +8686,7 @@
         <v>956</v>
       </c>
       <c r="E265" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.2">
@@ -8702,7 +8703,7 @@
         <v>956</v>
       </c>
       <c r="E266" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.2">
@@ -8719,7 +8720,7 @@
         <v>956</v>
       </c>
       <c r="E267" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.2">
@@ -8736,7 +8737,7 @@
         <v>956</v>
       </c>
       <c r="E268" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.2">
@@ -8753,7 +8754,7 @@
         <v>956</v>
       </c>
       <c r="E269" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.2">
@@ -8770,7 +8771,7 @@
         <v>956</v>
       </c>
       <c r="E270" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.2">
@@ -8787,7 +8788,7 @@
         <v>956</v>
       </c>
       <c r="E271" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.2">
@@ -8804,7 +8805,7 @@
         <v>956</v>
       </c>
       <c r="E272" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.2">
@@ -8821,7 +8822,7 @@
         <v>956</v>
       </c>
       <c r="E273" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.2">
@@ -8838,7 +8839,7 @@
         <v>956</v>
       </c>
       <c r="E274" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.2">
@@ -8855,7 +8856,7 @@
         <v>956</v>
       </c>
       <c r="E275" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.2">
@@ -8872,7 +8873,7 @@
         <v>956</v>
       </c>
       <c r="E276" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.2">
@@ -8889,7 +8890,7 @@
         <v>956</v>
       </c>
       <c r="E277" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.2">
@@ -8906,7 +8907,7 @@
         <v>956</v>
       </c>
       <c r="E278" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.2">
@@ -8923,7 +8924,7 @@
         <v>956</v>
       </c>
       <c r="E279" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.2">
@@ -8940,7 +8941,7 @@
         <v>956</v>
       </c>
       <c r="E280" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.2">
@@ -8957,7 +8958,7 @@
         <v>956</v>
       </c>
       <c r="E281" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.2">
@@ -8974,7 +8975,7 @@
         <v>956</v>
       </c>
       <c r="E282" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.2">
@@ -9005,7 +9006,7 @@
         <v>956</v>
       </c>
       <c r="E284" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.2">
@@ -9022,7 +9023,7 @@
         <v>956</v>
       </c>
       <c r="E285" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.2">
@@ -9039,7 +9040,7 @@
         <v>956</v>
       </c>
       <c r="E286" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.2">
@@ -9056,7 +9057,7 @@
         <v>956</v>
       </c>
       <c r="E287" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.2">
@@ -9073,7 +9074,7 @@
         <v>956</v>
       </c>
       <c r="E288" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.2">
@@ -9090,7 +9091,7 @@
         <v>956</v>
       </c>
       <c r="E289" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.2">
@@ -9107,7 +9108,7 @@
         <v>956</v>
       </c>
       <c r="E290" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.2">
@@ -9124,7 +9125,7 @@
         <v>956</v>
       </c>
       <c r="E291" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.2">
@@ -9141,7 +9142,7 @@
         <v>956</v>
       </c>
       <c r="E292" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.2">
@@ -9158,7 +9159,7 @@
         <v>956</v>
       </c>
       <c r="E293" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.2">
@@ -9175,7 +9176,7 @@
         <v>956</v>
       </c>
       <c r="E294" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.2">
@@ -9192,7 +9193,7 @@
         <v>956</v>
       </c>
       <c r="E295" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.2">
@@ -9209,7 +9210,7 @@
         <v>956</v>
       </c>
       <c r="E296" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.2">
@@ -9226,7 +9227,7 @@
         <v>956</v>
       </c>
       <c r="E297" s="2" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.2">
@@ -9243,7 +9244,7 @@
         <v>956</v>
       </c>
       <c r="E298" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.2">
@@ -9260,7 +9261,7 @@
         <v>956</v>
       </c>
       <c r="E299" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.2">
@@ -9277,7 +9278,7 @@
         <v>956</v>
       </c>
       <c r="E300" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.2">
@@ -9294,7 +9295,7 @@
         <v>956</v>
       </c>
       <c r="E301" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.2">
@@ -9311,7 +9312,7 @@
         <v>956</v>
       </c>
       <c r="E302" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.2">
@@ -9328,7 +9329,7 @@
         <v>956</v>
       </c>
       <c r="E303" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.2">
@@ -9345,7 +9346,7 @@
         <v>956</v>
       </c>
       <c r="E304" s="2" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.2">
@@ -9362,7 +9363,7 @@
         <v>956</v>
       </c>
       <c r="E305" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.2">
@@ -9379,7 +9380,7 @@
         <v>956</v>
       </c>
       <c r="E306" s="2" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.2">
@@ -9396,7 +9397,7 @@
         <v>956</v>
       </c>
       <c r="E307" s="2" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.2">
@@ -9413,7 +9414,7 @@
         <v>956</v>
       </c>
       <c r="E308" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.2">
@@ -9430,7 +9431,7 @@
         <v>956</v>
       </c>
       <c r="E309" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.2">
@@ -9447,7 +9448,7 @@
         <v>956</v>
       </c>
       <c r="E310" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.2">
@@ -9464,7 +9465,7 @@
         <v>956</v>
       </c>
       <c r="E311" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.2">
@@ -9481,7 +9482,7 @@
         <v>956</v>
       </c>
       <c r="E312" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.2">
@@ -9498,7 +9499,7 @@
         <v>956</v>
       </c>
       <c r="E313" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.2">
@@ -9515,7 +9516,7 @@
         <v>956</v>
       </c>
       <c r="E314" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.2">
@@ -9532,7 +9533,7 @@
         <v>956</v>
       </c>
       <c r="E315" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.2">
@@ -9549,7 +9550,7 @@
         <v>956</v>
       </c>
       <c r="E316" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.2">
@@ -9566,7 +9567,7 @@
         <v>956</v>
       </c>
       <c r="E317" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.2">
@@ -9583,7 +9584,7 @@
         <v>956</v>
       </c>
       <c r="E318" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.2">
@@ -9600,7 +9601,7 @@
         <v>956</v>
       </c>
       <c r="E319" s="16" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.2">
@@ -9617,7 +9618,7 @@
         <v>956</v>
       </c>
       <c r="E320" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.2">
@@ -9634,7 +9635,7 @@
         <v>956</v>
       </c>
       <c r="E321" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.2">
@@ -9651,7 +9652,7 @@
         <v>956</v>
       </c>
       <c r="E322" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.2">
@@ -9668,7 +9669,7 @@
         <v>956</v>
       </c>
       <c r="E323" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.2">
@@ -9685,7 +9686,7 @@
         <v>956</v>
       </c>
       <c r="E324" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.2">
@@ -9702,7 +9703,7 @@
         <v>956</v>
       </c>
       <c r="E325" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.2">
@@ -9719,7 +9720,7 @@
         <v>956</v>
       </c>
       <c r="E326" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.2">
@@ -9736,7 +9737,7 @@
         <v>956</v>
       </c>
       <c r="E327" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.2">
@@ -9753,7 +9754,7 @@
         <v>956</v>
       </c>
       <c r="E328" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.2">
@@ -9770,7 +9771,7 @@
         <v>956</v>
       </c>
       <c r="E329" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.2">
@@ -9787,7 +9788,7 @@
         <v>956</v>
       </c>
       <c r="E330" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.2">
@@ -9804,7 +9805,7 @@
         <v>956</v>
       </c>
       <c r="E331" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.2">
@@ -9821,7 +9822,7 @@
         <v>956</v>
       </c>
       <c r="E332" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.2">
@@ -9838,7 +9839,7 @@
         <v>956</v>
       </c>
       <c r="E333" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.2">
@@ -9855,7 +9856,7 @@
         <v>956</v>
       </c>
       <c r="E334" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.2">
@@ -9872,7 +9873,7 @@
         <v>956</v>
       </c>
       <c r="E335" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.2">
@@ -9889,7 +9890,7 @@
         <v>956</v>
       </c>
       <c r="E336" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.2">
@@ -9906,7 +9907,7 @@
         <v>956</v>
       </c>
       <c r="E337" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.2">
@@ -9923,7 +9924,7 @@
         <v>956</v>
       </c>
       <c r="E338" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.2">
@@ -9940,7 +9941,7 @@
         <v>956</v>
       </c>
       <c r="E339" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.2">
@@ -9957,7 +9958,7 @@
         <v>956</v>
       </c>
       <c r="E340" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.2">
@@ -9974,7 +9975,7 @@
         <v>956</v>
       </c>
       <c r="E341" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.2">
@@ -9991,7 +9992,7 @@
         <v>956</v>
       </c>
       <c r="E342" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.2">
@@ -10008,7 +10009,7 @@
         <v>956</v>
       </c>
       <c r="E343" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.2">
@@ -10025,7 +10026,7 @@
         <v>956</v>
       </c>
       <c r="E344" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.2">
@@ -10042,7 +10043,7 @@
         <v>956</v>
       </c>
       <c r="E345" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.2">
@@ -10059,7 +10060,7 @@
         <v>956</v>
       </c>
       <c r="E346" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.2">
@@ -10076,7 +10077,7 @@
         <v>956</v>
       </c>
       <c r="E347" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.2">
@@ -10093,7 +10094,7 @@
         <v>956</v>
       </c>
       <c r="E348" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.2">
@@ -10110,7 +10111,7 @@
         <v>956</v>
       </c>
       <c r="E349" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.2">
@@ -10127,7 +10128,7 @@
         <v>956</v>
       </c>
       <c r="E350" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.2">
@@ -10144,7 +10145,7 @@
         <v>956</v>
       </c>
       <c r="E351" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.2">
@@ -10161,7 +10162,7 @@
         <v>956</v>
       </c>
       <c r="E352" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.2">
@@ -10178,7 +10179,7 @@
         <v>956</v>
       </c>
       <c r="E353" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.2">
@@ -10195,7 +10196,7 @@
         <v>956</v>
       </c>
       <c r="E354" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.2">
@@ -10212,7 +10213,7 @@
         <v>956</v>
       </c>
       <c r="E355" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.2">
@@ -10229,7 +10230,7 @@
         <v>956</v>
       </c>
       <c r="E356" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.2">
@@ -10246,7 +10247,7 @@
         <v>956</v>
       </c>
       <c r="E357" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.2">
@@ -10263,7 +10264,7 @@
         <v>956</v>
       </c>
       <c r="E358" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.2">
@@ -10280,7 +10281,7 @@
         <v>956</v>
       </c>
       <c r="E359" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.2">
@@ -10297,7 +10298,7 @@
         <v>956</v>
       </c>
       <c r="E360" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.2">
@@ -10314,7 +10315,7 @@
         <v>956</v>
       </c>
       <c r="E361" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.2">
@@ -10331,7 +10332,7 @@
         <v>956</v>
       </c>
       <c r="E362" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.2">
@@ -10348,7 +10349,7 @@
         <v>956</v>
       </c>
       <c r="E363" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.2">
@@ -10365,7 +10366,7 @@
         <v>956</v>
       </c>
       <c r="E364" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.2">
@@ -10382,7 +10383,7 @@
         <v>956</v>
       </c>
       <c r="E365" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.2">
@@ -10399,7 +10400,7 @@
         <v>956</v>
       </c>
       <c r="E366" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.2">
@@ -10416,7 +10417,7 @@
         <v>956</v>
       </c>
       <c r="E367" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.2">
@@ -10433,7 +10434,7 @@
         <v>956</v>
       </c>
       <c r="E368" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.2">
@@ -10450,7 +10451,7 @@
         <v>956</v>
       </c>
       <c r="E369" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.2">
@@ -10467,7 +10468,7 @@
         <v>956</v>
       </c>
       <c r="E370" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.2">
@@ -10484,7 +10485,7 @@
         <v>956</v>
       </c>
       <c r="E371" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.2">
@@ -10501,7 +10502,7 @@
         <v>956</v>
       </c>
       <c r="E372" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.2">
@@ -10518,7 +10519,7 @@
         <v>956</v>
       </c>
       <c r="E373" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.2">
@@ -10535,7 +10536,7 @@
         <v>956</v>
       </c>
       <c r="E374" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.2">
@@ -10552,7 +10553,7 @@
         <v>956</v>
       </c>
       <c r="E375" s="2" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.2">
@@ -10569,7 +10570,7 @@
         <v>956</v>
       </c>
       <c r="E376" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.2">
@@ -10586,7 +10587,7 @@
         <v>956</v>
       </c>
       <c r="E377" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.2">
@@ -10603,7 +10604,7 @@
         <v>956</v>
       </c>
       <c r="E378" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.2">
@@ -10620,7 +10621,7 @@
         <v>956</v>
       </c>
       <c r="E379" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.2">
@@ -10637,7 +10638,7 @@
         <v>956</v>
       </c>
       <c r="E380" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.2">
@@ -10654,7 +10655,7 @@
         <v>956</v>
       </c>
       <c r="E381" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.2">
@@ -10671,7 +10672,7 @@
         <v>956</v>
       </c>
       <c r="E382" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.2">
@@ -10688,7 +10689,7 @@
         <v>956</v>
       </c>
       <c r="E383" s="2" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.2">
@@ -10705,7 +10706,7 @@
         <v>956</v>
       </c>
       <c r="E384" s="2" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.2">
@@ -10722,7 +10723,7 @@
         <v>956</v>
       </c>
       <c r="E385" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.2">
@@ -10739,7 +10740,7 @@
         <v>956</v>
       </c>
       <c r="E386" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.2">
@@ -10756,7 +10757,7 @@
         <v>956</v>
       </c>
       <c r="E387" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.2">
@@ -10773,7 +10774,7 @@
         <v>956</v>
       </c>
       <c r="E388" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.2">
@@ -10790,7 +10791,7 @@
         <v>956</v>
       </c>
       <c r="E389" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.2">
@@ -10807,7 +10808,7 @@
         <v>956</v>
       </c>
       <c r="E390" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.2">
@@ -10824,7 +10825,7 @@
         <v>956</v>
       </c>
       <c r="E391" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.2">
@@ -10841,7 +10842,7 @@
         <v>956</v>
       </c>
       <c r="E392" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.2">
@@ -10858,7 +10859,7 @@
         <v>956</v>
       </c>
       <c r="E393" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.2">
@@ -10875,7 +10876,7 @@
         <v>956</v>
       </c>
       <c r="E394" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.2">
@@ -10892,7 +10893,7 @@
         <v>956</v>
       </c>
       <c r="E395" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.2">
@@ -10909,7 +10910,7 @@
         <v>956</v>
       </c>
       <c r="E396" s="17" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.2">
@@ -10926,7 +10927,7 @@
         <v>956</v>
       </c>
       <c r="E397" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.2">
@@ -10943,7 +10944,7 @@
         <v>956</v>
       </c>
       <c r="E398" s="20" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.2">
@@ -10960,7 +10961,7 @@
         <v>956</v>
       </c>
       <c r="E399" s="20" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.2">
@@ -10977,7 +10978,7 @@
         <v>956</v>
       </c>
       <c r="E400" s="20" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.2">
@@ -10994,7 +10995,7 @@
         <v>956</v>
       </c>
       <c r="E401" s="20" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.2">
@@ -11011,7 +11012,7 @@
         <v>956</v>
       </c>
       <c r="E402" s="20" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.2">
@@ -11028,7 +11029,7 @@
         <v>956</v>
       </c>
       <c r="E403" s="20" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.2">
@@ -11045,7 +11046,7 @@
         <v>956</v>
       </c>
       <c r="E404" s="20" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.2">
@@ -11062,7 +11063,7 @@
         <v>956</v>
       </c>
       <c r="E405" s="20" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.2">
@@ -11079,7 +11080,7 @@
         <v>956</v>
       </c>
       <c r="E406" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="407" spans="1:5" x14ac:dyDescent="0.2">
@@ -11096,7 +11097,7 @@
         <v>956</v>
       </c>
       <c r="E407" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.2">
@@ -11113,7 +11114,7 @@
         <v>956</v>
       </c>
       <c r="E408" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.2">
@@ -11130,7 +11131,7 @@
         <v>956</v>
       </c>
       <c r="E409" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.2">
@@ -11147,7 +11148,7 @@
         <v>956</v>
       </c>
       <c r="E410" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.2">
@@ -11164,7 +11165,7 @@
         <v>956</v>
       </c>
       <c r="E411" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.2">
@@ -11181,7 +11182,7 @@
         <v>956</v>
       </c>
       <c r="E412" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.2">
@@ -11198,7 +11199,7 @@
         <v>956</v>
       </c>
       <c r="E413" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.2">
@@ -11215,7 +11216,7 @@
         <v>956</v>
       </c>
       <c r="E414" s="20" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.2">
@@ -11232,7 +11233,7 @@
         <v>956</v>
       </c>
       <c r="E415" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.2">
@@ -11249,7 +11250,7 @@
         <v>956</v>
       </c>
       <c r="E416" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="417" spans="1:5" x14ac:dyDescent="0.2">
@@ -11266,7 +11267,7 @@
         <v>956</v>
       </c>
       <c r="E417" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="418" spans="1:5" x14ac:dyDescent="0.2">
@@ -11283,7 +11284,7 @@
         <v>956</v>
       </c>
       <c r="E418" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="419" spans="1:5" x14ac:dyDescent="0.2">
@@ -11330,7 +11331,7 @@
         <v>956</v>
       </c>
       <c r="E421" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.2">
@@ -11347,7 +11348,7 @@
         <v>955</v>
       </c>
       <c r="E422" s="21" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.2">
@@ -11364,7 +11365,7 @@
         <v>955</v>
       </c>
       <c r="E423" s="21" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.2">
@@ -11411,7 +11412,7 @@
         <v>956</v>
       </c>
       <c r="E426" s="7" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.2">
@@ -11428,7 +11429,7 @@
         <v>956</v>
       </c>
       <c r="E427" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.2">
@@ -11445,7 +11446,7 @@
         <v>956</v>
       </c>
       <c r="E428" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.2">
@@ -11462,7 +11463,7 @@
         <v>956</v>
       </c>
       <c r="E429" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.2">
@@ -11479,7 +11480,7 @@
         <v>956</v>
       </c>
       <c r="E430" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.2">
@@ -11496,7 +11497,7 @@
         <v>956</v>
       </c>
       <c r="E431" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.2">
@@ -11513,7 +11514,7 @@
         <v>956</v>
       </c>
       <c r="E432" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="433" spans="1:5" x14ac:dyDescent="0.2">
@@ -11530,7 +11531,7 @@
         <v>956</v>
       </c>
       <c r="E433" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="434" spans="1:5" x14ac:dyDescent="0.2">
@@ -11547,7 +11548,7 @@
         <v>956</v>
       </c>
       <c r="E434" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="435" spans="1:5" x14ac:dyDescent="0.2">
@@ -11564,7 +11565,7 @@
         <v>956</v>
       </c>
       <c r="E435" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="436" spans="1:5" x14ac:dyDescent="0.2">
@@ -11581,7 +11582,7 @@
         <v>956</v>
       </c>
       <c r="E436" s="7" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.2">
@@ -11598,7 +11599,7 @@
         <v>956</v>
       </c>
       <c r="E437" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.2">
@@ -11615,7 +11616,7 @@
         <v>956</v>
       </c>
       <c r="E438" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="439" spans="1:5" x14ac:dyDescent="0.2">
@@ -11632,7 +11633,7 @@
         <v>956</v>
       </c>
       <c r="E439" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.2">
@@ -11649,7 +11650,7 @@
         <v>956</v>
       </c>
       <c r="E440" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="441" spans="1:5" x14ac:dyDescent="0.2">
@@ -11666,7 +11667,7 @@
         <v>956</v>
       </c>
       <c r="E441" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.2">
@@ -11683,7 +11684,7 @@
         <v>956</v>
       </c>
       <c r="E442" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="443" spans="1:5" x14ac:dyDescent="0.2">
@@ -11700,7 +11701,7 @@
         <v>956</v>
       </c>
       <c r="E443" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="444" spans="1:5" x14ac:dyDescent="0.2">
@@ -11717,7 +11718,7 @@
         <v>956</v>
       </c>
       <c r="E444" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="445" spans="1:5" x14ac:dyDescent="0.2">
@@ -11734,7 +11735,7 @@
         <v>956</v>
       </c>
       <c r="E445" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.2">
@@ -11751,7 +11752,7 @@
         <v>956</v>
       </c>
       <c r="E446" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="447" spans="1:5" x14ac:dyDescent="0.2">
@@ -11768,7 +11769,7 @@
         <v>956</v>
       </c>
       <c r="E447" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.2">
@@ -11785,7 +11786,7 @@
         <v>956</v>
       </c>
       <c r="E448" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.2">
@@ -11802,7 +11803,7 @@
         <v>956</v>
       </c>
       <c r="E449" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.2">
@@ -11819,7 +11820,7 @@
         <v>956</v>
       </c>
       <c r="E450" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="451" spans="1:5" x14ac:dyDescent="0.2">
@@ -11836,7 +11837,7 @@
         <v>956</v>
       </c>
       <c r="E451" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="452" spans="1:5" x14ac:dyDescent="0.2">
@@ -11853,7 +11854,7 @@
         <v>956</v>
       </c>
       <c r="E452" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="453" spans="1:5" x14ac:dyDescent="0.2">
@@ -11870,7 +11871,7 @@
         <v>956</v>
       </c>
       <c r="E453" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="454" spans="1:5" x14ac:dyDescent="0.2">
@@ -11887,7 +11888,7 @@
         <v>956</v>
       </c>
       <c r="E454" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="455" spans="1:5" x14ac:dyDescent="0.2">
@@ -11904,7 +11905,7 @@
         <v>956</v>
       </c>
       <c r="E455" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="456" spans="1:5" x14ac:dyDescent="0.2">
@@ -11921,7 +11922,7 @@
         <v>956</v>
       </c>
       <c r="E456" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="457" spans="1:5" x14ac:dyDescent="0.2">
@@ -11938,7 +11939,7 @@
         <v>956</v>
       </c>
       <c r="E457" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="458" spans="1:5" x14ac:dyDescent="0.2">
@@ -11955,7 +11956,7 @@
         <v>956</v>
       </c>
       <c r="E458" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.2">
@@ -11972,7 +11973,7 @@
         <v>956</v>
       </c>
       <c r="E459" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="460" spans="1:5" x14ac:dyDescent="0.2">
@@ -11989,7 +11990,7 @@
         <v>956</v>
       </c>
       <c r="E460" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="461" spans="1:5" x14ac:dyDescent="0.2">
@@ -12006,7 +12007,7 @@
         <v>956</v>
       </c>
       <c r="E461" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="462" spans="1:5" x14ac:dyDescent="0.2">
@@ -12023,7 +12024,7 @@
         <v>956</v>
       </c>
       <c r="E462" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="463" spans="1:5" x14ac:dyDescent="0.2">
@@ -12040,7 +12041,7 @@
         <v>956</v>
       </c>
       <c r="E463" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.2">
@@ -12057,7 +12058,7 @@
         <v>956</v>
       </c>
       <c r="E464" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="465" spans="1:5" x14ac:dyDescent="0.2">
@@ -12074,7 +12075,7 @@
         <v>956</v>
       </c>
       <c r="E465" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="466" spans="1:5" x14ac:dyDescent="0.2">
@@ -12091,7 +12092,7 @@
         <v>956</v>
       </c>
       <c r="E466" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="467" spans="1:5" x14ac:dyDescent="0.2">
@@ -12108,7 +12109,7 @@
         <v>956</v>
       </c>
       <c r="E467" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="468" spans="1:5" x14ac:dyDescent="0.2">
@@ -12125,7 +12126,7 @@
         <v>956</v>
       </c>
       <c r="E468" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="469" spans="1:5" x14ac:dyDescent="0.2">
@@ -12142,7 +12143,7 @@
         <v>956</v>
       </c>
       <c r="E469" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="470" spans="1:5" x14ac:dyDescent="0.2">
@@ -12159,7 +12160,7 @@
         <v>956</v>
       </c>
       <c r="E470" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.2">
@@ -12176,7 +12177,7 @@
         <v>956</v>
       </c>
       <c r="E471" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="472" spans="1:5" x14ac:dyDescent="0.2">
@@ -12193,7 +12194,7 @@
         <v>956</v>
       </c>
       <c r="E472" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="473" spans="1:5" x14ac:dyDescent="0.2">
@@ -12210,7 +12211,7 @@
         <v>956</v>
       </c>
       <c r="E473" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="474" spans="1:5" x14ac:dyDescent="0.2">
@@ -12227,7 +12228,7 @@
         <v>956</v>
       </c>
       <c r="E474" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="475" spans="1:5" x14ac:dyDescent="0.2">
@@ -12244,7 +12245,7 @@
         <v>956</v>
       </c>
       <c r="E475" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="476" spans="1:5" x14ac:dyDescent="0.2">
@@ -12261,7 +12262,7 @@
         <v>956</v>
       </c>
       <c r="E476" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.2">
@@ -12278,7 +12279,7 @@
         <v>956</v>
       </c>
       <c r="E477" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="478" spans="1:5" x14ac:dyDescent="0.2">
@@ -12295,7 +12296,7 @@
         <v>956</v>
       </c>
       <c r="E478" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.2">
@@ -12312,7 +12313,7 @@
         <v>956</v>
       </c>
       <c r="E479" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="480" spans="1:5" x14ac:dyDescent="0.2">
@@ -12329,7 +12330,7 @@
         <v>956</v>
       </c>
       <c r="E480" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="481" spans="1:5" x14ac:dyDescent="0.2">
@@ -12346,7 +12347,7 @@
         <v>956</v>
       </c>
       <c r="E481" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="482" spans="1:5" x14ac:dyDescent="0.2">
@@ -12363,7 +12364,7 @@
         <v>956</v>
       </c>
       <c r="E482" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="483" spans="1:5" x14ac:dyDescent="0.2">
@@ -12380,7 +12381,7 @@
         <v>956</v>
       </c>
       <c r="E483" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="484" spans="1:5" x14ac:dyDescent="0.2">
@@ -12397,7 +12398,7 @@
         <v>956</v>
       </c>
       <c r="E484" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.2">
@@ -12414,7 +12415,7 @@
         <v>956</v>
       </c>
       <c r="E485" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.2">
@@ -12431,7 +12432,7 @@
         <v>956</v>
       </c>
       <c r="E486" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="487" spans="1:5" x14ac:dyDescent="0.2">
@@ -12448,7 +12449,7 @@
         <v>956</v>
       </c>
       <c r="E487" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="488" spans="1:5" x14ac:dyDescent="0.2">
@@ -12465,7 +12466,7 @@
         <v>956</v>
       </c>
       <c r="E488" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="489" spans="1:5" x14ac:dyDescent="0.2">
@@ -12482,7 +12483,7 @@
         <v>956</v>
       </c>
       <c r="E489" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="490" spans="1:5" x14ac:dyDescent="0.2">
@@ -12499,7 +12500,7 @@
         <v>956</v>
       </c>
       <c r="E490" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.2">
@@ -12516,7 +12517,7 @@
         <v>956</v>
       </c>
       <c r="E491" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.2">
@@ -12533,7 +12534,7 @@
         <v>956</v>
       </c>
       <c r="E492" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="493" spans="1:5" x14ac:dyDescent="0.2">
@@ -12550,7 +12551,7 @@
         <v>956</v>
       </c>
       <c r="E493" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.2">
@@ -12567,7 +12568,7 @@
         <v>956</v>
       </c>
       <c r="E494" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="495" spans="1:5" x14ac:dyDescent="0.2">
@@ -12584,7 +12585,7 @@
         <v>956</v>
       </c>
       <c r="E495" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.2">
@@ -12601,7 +12602,7 @@
         <v>956</v>
       </c>
       <c r="E496" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.2">
@@ -12618,7 +12619,7 @@
         <v>956</v>
       </c>
       <c r="E497" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="498" spans="1:5" x14ac:dyDescent="0.2">
@@ -12635,7 +12636,7 @@
         <v>956</v>
       </c>
       <c r="E498" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="499" spans="1:5" x14ac:dyDescent="0.2">
@@ -12652,7 +12653,7 @@
         <v>956</v>
       </c>
       <c r="E499" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.2">
@@ -12669,7 +12670,7 @@
         <v>956</v>
       </c>
       <c r="E500" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="501" spans="1:5" x14ac:dyDescent="0.2">
@@ -12686,7 +12687,7 @@
         <v>956</v>
       </c>
       <c r="E501" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="502" spans="1:5" x14ac:dyDescent="0.2">
@@ -12703,7 +12704,7 @@
         <v>956</v>
       </c>
       <c r="E502" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="503" spans="1:5" x14ac:dyDescent="0.2">
@@ -12720,7 +12721,7 @@
         <v>956</v>
       </c>
       <c r="E503" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="504" spans="1:5" x14ac:dyDescent="0.2">
@@ -12737,7 +12738,7 @@
         <v>956</v>
       </c>
       <c r="E504" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.2">
@@ -12754,7 +12755,7 @@
         <v>956</v>
       </c>
       <c r="E505" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.2">
@@ -12771,7 +12772,7 @@
         <v>956</v>
       </c>
       <c r="E506" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.2">
@@ -12788,7 +12789,7 @@
         <v>956</v>
       </c>
       <c r="E507" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.2">
@@ -12805,7 +12806,7 @@
         <v>956</v>
       </c>
       <c r="E508" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.2">
@@ -12822,7 +12823,7 @@
         <v>956</v>
       </c>
       <c r="E509" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.2">
@@ -12839,7 +12840,7 @@
         <v>956</v>
       </c>
       <c r="E510" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.2">
@@ -12856,7 +12857,7 @@
         <v>956</v>
       </c>
       <c r="E511" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.2">
@@ -12873,7 +12874,7 @@
         <v>956</v>
       </c>
       <c r="E512" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.2">
@@ -13262,7 +13263,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView topLeftCell="B6" workbookViewId="0">
@@ -13278,19 +13279,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>999</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>1000</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>1001</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
+        <v>1000</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>1002</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>1001</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>1003</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -13307,7 +13308,7 @@
         <v>473</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -13324,7 +13325,7 @@
         <v>693</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -13341,7 +13342,7 @@
         <v>695</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -13358,7 +13359,7 @@
         <v>697</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -13375,7 +13376,7 @@
         <v>699</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -13392,7 +13393,7 @@
         <v>557</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13409,7 +13410,7 @@
         <v>702</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -13426,7 +13427,7 @@
         <v>561</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -13443,7 +13444,7 @@
         <v>705</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -13460,7 +13461,7 @@
         <v>707</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -13477,7 +13478,7 @@
         <v>709</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -13494,7 +13495,7 @@
         <v>711</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -13511,7 +13512,7 @@
         <v>571</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -13528,7 +13529,7 @@
         <v>714</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -13545,7 +13546,7 @@
         <v>575</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -13562,7 +13563,7 @@
         <v>717</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -13579,7 +13580,7 @@
         <v>719</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -13596,7 +13597,7 @@
         <v>581</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -13613,7 +13614,7 @@
         <v>583</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -13630,7 +13631,7 @@
         <v>585</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -13647,7 +13648,7 @@
         <v>587</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -13660,7 +13661,7 @@
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="19" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -13677,7 +13678,7 @@
         <v>591</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13728,7 +13729,7 @@
         <v>597</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -13745,7 +13746,7 @@
         <v>599</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -13762,7 +13763,7 @@
         <v>601</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -13779,7 +13780,7 @@
         <v>603</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -13796,7 +13797,7 @@
         <v>605</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -13813,7 +13814,7 @@
         <v>607</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -13830,7 +13831,7 @@
         <v>734</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -13847,7 +13848,7 @@
         <v>736</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -13864,7 +13865,7 @@
         <v>738</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -13881,7 +13882,7 @@
         <v>740</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -13898,7 +13899,7 @@
         <v>617</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -13915,7 +13916,7 @@
         <v>619</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spurious correlation and simdata work
</commit_message>
<xml_diff>
--- a/internal_datamap_files/liftPR_internal_covar_map.xlsx
+++ b/internal_datamap_files/liftPR_internal_covar_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/internal_datamap_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D8D744-0D15-D547-ABAF-E6DC26AB92E1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4616B9-A250-FD48-9C66-AD0CE80E3D90}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5340" yWindow="460" windowWidth="20200" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4291,7 +4291,7 @@
   <dimension ref="A1:E538"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
explore interaction between wealth and urbanicity in the pv data
</commit_message>
<xml_diff>
--- a/internal_datamap_files/liftPR_internal_covar_map.xlsx
+++ b/internal_datamap_files/liftPR_internal_covar_map.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/internal_datamap_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4616B9-A250-FD48-9C66-AD0CE80E3D90}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA51BA0-0885-B341-A7A1-1469A7B0D978}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="460" windowWidth="20200" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2620" yWindow="460" windowWidth="20200" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
     <sheet name="covar_names_labels" sheetId="1" r:id="rId2"/>
     <sheet name="cmpr_M_F_biocovar" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -4290,8 +4290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E538"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="B231" sqref="B231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4794,20 +4794,20 @@
         <v>967</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C32" t="s">
-        <v>956</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C32" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>965</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="2" t="s">
         <v>968</v>
       </c>
     </row>
@@ -13266,7 +13266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>

</xml_diff>